<commit_message>
fix philip airlines bsp
</commit_message>
<xml_diff>
--- a/Data/Config Prod.xlsx
+++ b/Data/Config Prod.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TVLK\Sprint 3\Traveloka_DataAutomation_Performer_Email_S3\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tvlk\Email Sprint 3\Traveloka_DataAutomation_Performer_Email_S3\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545DADF6-CAAF-4B44-8848-048E9699B6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418650B5-7386-485D-B3F7-2BD7933874D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="165" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -226,6 +226,12 @@
   </si>
   <si>
     <t>AutoRetrySchedule</t>
+  </si>
+  <si>
+    <t>PathTabula</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathTabula</t>
   </si>
 </sst>
 </file>
@@ -607,12 +613,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -660,7 +666,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -670,7 +676,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1717,12 +1723,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1759,7 +1765,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1770,7 +1776,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1884,7 +1890,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -2880,12 +2886,12 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2980,7 +2986,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>